<commit_message>
añadidos en el init excepciones de negocio y de sistema
</commit_message>
<xml_diff>
--- a/Data/Clientes/Finanzas.xlsx
+++ b/Data/Clientes/Finanzas.xlsx
@@ -2984,13 +2984,13 @@
         <v>Jefe de equipo de Organizacion en el area de Organizacion y Operaciones</v>
       </c>
       <c r="C96" t="str">
-        <v>Evo Banco</v>
+        <v>EVO Banco</v>
       </c>
       <c r="E96" t="str">
         <v>btamayo@evobanco.com</v>
       </c>
       <c r="H96">
-        <v>1402</v>
+        <v>4313</v>
       </c>
       <c r="I96">
         <v>4187</v>
@@ -6380,13 +6380,13 @@
         <v>Responsable Operaciones EVO Banco</v>
       </c>
       <c r="C222" t="str">
-        <v>Evo Banco</v>
+        <v>EVO Banco</v>
       </c>
       <c r="E222" t="str">
         <v>fcedenilla@evobanco.com</v>
       </c>
       <c r="H222">
-        <v>1402</v>
+        <v>4313</v>
       </c>
       <c r="I222">
         <v>4202</v>
@@ -6785,13 +6785,13 @@
         <v>Innovacion Disruptiva</v>
       </c>
       <c r="C237" t="str">
-        <v>Evo Banco</v>
+        <v>EVO Banco</v>
       </c>
       <c r="E237" t="str">
         <v>gblasco@evobanco.com</v>
       </c>
       <c r="H237">
-        <v>1402</v>
+        <v>4313</v>
       </c>
       <c r="I237">
         <v>4277</v>
@@ -7260,13 +7260,13 @@
         <v>Especialista de innovación disruptiva</v>
       </c>
       <c r="C254" t="str">
-        <v>Evo Banco</v>
+        <v>EVO Banco</v>
       </c>
       <c r="E254" t="str">
         <v>iizquierdo@evobanco.com</v>
       </c>
       <c r="H254">
-        <v>1402</v>
+        <v>4313</v>
       </c>
       <c r="I254">
         <v>4044</v>
@@ -8282,13 +8282,13 @@
         <v>Chief Innovation Officer. Director Corporativo Innovación y Analítica Avanzada.</v>
       </c>
       <c r="C291" t="str">
-        <v>Evo Banco</v>
+        <v>EVO Banco</v>
       </c>
       <c r="E291" t="str">
         <v>jgonzalez@evobanco.com</v>
       </c>
       <c r="H291">
-        <v>1402</v>
+        <v>4313</v>
       </c>
       <c r="I291">
         <v>4076</v>
@@ -8959,13 +8959,13 @@
         <v>Director ejecutivo de operaciones</v>
       </c>
       <c r="C316" t="str">
-        <v>Evo Banco</v>
+        <v>EVO Banco</v>
       </c>
       <c r="E316" t="str">
         <v>jandreo@evobanco.com</v>
       </c>
       <c r="H316">
-        <v>1402</v>
+        <v>4313</v>
       </c>
       <c r="I316">
         <v>4195</v>
@@ -14269,13 +14269,13 @@
         <v>Director of Disruptive Innovation and Advanced Analytics</v>
       </c>
       <c r="C511" t="str">
-        <v>Evo Banco</v>
+        <v>EVO Banco</v>
       </c>
       <c r="E511" t="str">
         <v>ptome@evobanco.com</v>
       </c>
       <c r="H511">
-        <v>1402</v>
+        <v>4313</v>
       </c>
       <c r="I511">
         <v>4090</v>

</xml_diff>